<commit_message>
SN: TIDC coverage survey, update sile list
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/Oncho/Mai 2021/bf_ect_Oncho_2_couverture_202105.xlsx
+++ b/Coverage Survey/Burkina Faso/Oncho/Mai 2021/bf_ect_Oncho_2_couverture_202105.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Burkina Faso\Oncho\March 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Burkina Faso\Oncho\Mai 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{36B9A701-2685-402F-8125-50E81BD753B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE3177E-9008-456C-B209-FDAF21AC4E3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterate="1" iterateCount="1000" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -576,12 +576,6 @@
     <t>Traitement_par_lequipe</t>
   </si>
   <si>
-    <t>(BF - Avril 2021) - ECT TIDC Oncho 2021 - 2. Formulaire Couverture 2021</t>
-  </si>
-  <si>
-    <t>bf_ect_Oncho_2_couverture_202104</t>
-  </si>
-  <si>
     <t>list_lieu_menage</t>
   </si>
   <si>
@@ -601,12 +595,18 @@
   </si>
   <si>
     <t>CSPS</t>
+  </si>
+  <si>
+    <t>bf_ect_Oncho_2_couverture_202105</t>
+  </si>
+  <si>
+    <t>(BF - Mai 2021) - ECT TIDC Oncho 2021 - 2. Formulaire Couverture 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1011,13 +1011,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1094,10 +1094,10 @@
         <v>174</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>78</v>
@@ -1190,7 +1190,7 @@
         <v>172</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>15</v>
@@ -1273,7 +1273,7 @@
         <v>138</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>139</v>
@@ -1583,13 +1583,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>39</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>95</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>90</v>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>91</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>48</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>92</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>93</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>46</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>94</v>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>164</v>
@@ -2098,18 +2098,18 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>165</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>166</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>167</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>163</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>162</v>
@@ -2174,21 +2174,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2207,13 +2207,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>185</v>
+        <v>192</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="C2" s="9">
-        <v>20210329</v>
+        <v>20210421</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>135</v>

</xml_diff>